<commit_message>
Added some more areas
</commit_message>
<xml_diff>
--- a/directional_areas.xlsx
+++ b/directional_areas.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviauddin/Documents/Agency fMRI/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="880" yWindow="0" windowWidth="24540" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="1360" yWindow="460" windowWidth="24540" windowHeight="15020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="leveraging" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="49">
   <si>
     <t>contrast</t>
   </si>
@@ -141,6 +146,33 @@
   </si>
   <si>
     <t>R anterior temporal</t>
+  </si>
+  <si>
+    <t>L precuneus, extending to L IP sulcus</t>
+  </si>
+  <si>
+    <t>R IP sulcus</t>
+  </si>
+  <si>
+    <t>L cuneus/middle occipital gyrus</t>
+  </si>
+  <si>
+    <t>R STS/middle temporal gyrus</t>
+  </si>
+  <si>
+    <t>R angular gyrus/inferior parietal</t>
+  </si>
+  <si>
+    <t>R posterior fusiform</t>
+  </si>
+  <si>
+    <t>L middle occipital gyrus</t>
+  </si>
+  <si>
+    <t>R inferior occipital gyrus</t>
+  </si>
+  <si>
+    <t>L IP sulcus</t>
   </si>
 </sst>
 </file>
@@ -212,13 +244,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -226,12 +254,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -559,11 +598,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" customWidth="1"/>
@@ -576,27 +615,27 @@
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="1"/>
@@ -604,42 +643,42 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="5" customFormat="1">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="5">
+    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
         <v>-18</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="3">
         <v>28</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="3">
         <v>0</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>-18</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <v>24</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="3">
         <v>11106</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="3">
         <v>0</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -674,7 +713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -699,17 +738,17 @@
       <c r="H4">
         <v>26</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -741,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -773,7 +812,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -798,14 +837,14 @@
       <c r="H7">
         <v>20</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J7">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -837,899 +876,1142 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6">
-        <v>6</v>
-      </c>
-      <c r="C9" s="6">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4">
         <v>4</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>44</v>
       </c>
-      <c r="E9" s="6">
-        <v>6</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="E9" s="4">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4">
         <v>5</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <v>40</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="4">
         <v>19</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="4">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="6">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4">
         <v>18</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>24</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>44</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="4">
         <v>18</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="4">
         <v>26</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="4">
         <v>41</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="4">
         <v>10</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="6">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4">
         <v>-16</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>-20</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>-10</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <v>-15</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="4">
         <v>-21</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="4">
         <v>-4</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="4">
         <v>13</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="6">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4">
         <v>-16</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>-10</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>24</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>-15</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="4">
         <v>-10</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <v>23</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="4">
         <v>5</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="6">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4">
         <v>24</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>12</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="4">
         <v>46</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="4">
         <v>24</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="4">
         <v>14</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="4">
         <v>43</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="4">
         <v>19</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="6">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4">
         <v>14</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>38</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="4">
         <v>-12</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="4">
         <v>13</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="4">
         <v>33</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="4">
         <v>-10</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="4">
         <v>12</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="6">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4">
         <v>28</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <v>10</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="4">
         <v>8</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="4">
         <v>27</v>
       </c>
-      <c r="F15" s="6">
-        <v>7</v>
-      </c>
-      <c r="G15" s="6">
+      <c r="F15" s="4">
+        <v>7</v>
+      </c>
+      <c r="G15" s="4">
         <v>10</v>
       </c>
-      <c r="H15" s="6">
-        <v>7</v>
-      </c>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="4">
+        <v>7</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="4">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="6">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4">
         <v>-42</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="4">
         <v>-16</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="4">
         <v>34</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="4">
         <v>-41</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="4">
         <v>-15</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="4">
         <v>32</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="4">
         <v>9</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="6">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4">
         <v>2</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="4">
         <v>10</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="4">
         <v>48</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="4">
         <v>2</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="4">
         <v>12</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="4">
         <v>44</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="4">
         <v>11</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="6">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="4">
         <v>-44</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="4">
         <v>46</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="4">
         <v>18</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="4">
         <v>-43</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="4">
         <v>45</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="4">
         <v>17</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="4">
         <v>14</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="4">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="6">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4">
         <v>26</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="4">
         <v>40</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="4">
         <v>40</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="4">
         <v>26</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="4">
         <v>41</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="4">
         <v>37</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="4">
         <v>10</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="4">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="6">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4">
         <v>-46</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="4">
         <v>14</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="4">
         <v>24</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="4">
         <v>-44</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="4">
         <v>13</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="4">
         <v>24</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="4">
         <v>15</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="4">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="6">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4">
         <v>46</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="4">
         <v>2</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="4">
         <v>-30</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="4">
         <v>44</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="4">
         <v>-2</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="4">
         <v>-22</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="4">
         <v>17</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="4">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="6">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="4">
         <v>38</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="4">
         <v>-2</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="4">
         <v>16</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="4">
         <v>36</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="4">
         <v>-3</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="4">
         <v>17</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="4">
         <v>8</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="4">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="6">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4">
         <v>-20</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="4">
         <v>-10</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="4">
         <v>10</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="4">
         <v>-19</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="4">
         <v>-11</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="4">
         <v>11</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="4">
         <v>5</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="6">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="4">
         <v>32</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="4">
         <v>-2</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="4">
         <v>-30</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="4">
         <v>31</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="4">
         <v>-5</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="4">
         <v>-22</v>
       </c>
-      <c r="H24" s="6">
-        <v>6</v>
-      </c>
-      <c r="I24" s="6" t="s">
+      <c r="H24" s="4">
+        <v>6</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="4">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="6">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="4">
         <v>-34</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="4">
         <v>48</v>
       </c>
-      <c r="D25" s="6">
-        <v>6</v>
-      </c>
-      <c r="E25" s="6">
+      <c r="D25" s="4">
+        <v>6</v>
+      </c>
+      <c r="E25" s="4">
         <v>-34</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="4">
         <v>45</v>
       </c>
-      <c r="G25" s="6">
-        <v>6</v>
-      </c>
-      <c r="H25" s="6">
+      <c r="G25" s="4">
+        <v>6</v>
+      </c>
+      <c r="H25" s="4">
         <v>5</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25" s="4">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="6">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="4">
         <v>-26</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="4">
         <v>50</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <v>18</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="4">
         <v>-26</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="4">
         <v>48</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="4">
         <v>16</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="4">
         <v>10</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J26" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="6">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="4">
         <v>24</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="4">
         <v>8</v>
       </c>
-      <c r="D27" s="6">
-        <v>6</v>
-      </c>
-      <c r="E27" s="6">
+      <c r="D27" s="4">
+        <v>6</v>
+      </c>
+      <c r="E27" s="4">
         <v>23</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="4">
         <v>5</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="4">
         <v>8</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="4">
         <v>9</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="4">
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="6">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="4">
         <v>-6</v>
       </c>
-      <c r="C28" s="6">
-        <v>6</v>
-      </c>
-      <c r="D28" s="6">
+      <c r="C28" s="4">
+        <v>6</v>
+      </c>
+      <c r="D28" s="4">
         <v>46</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="4">
         <v>-5</v>
       </c>
-      <c r="F28" s="6">
-        <v>7</v>
-      </c>
-      <c r="G28" s="6">
+      <c r="F28" s="4">
+        <v>7</v>
+      </c>
+      <c r="G28" s="4">
         <v>42</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="4">
         <v>5</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="I28" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J28" s="6">
+      <c r="J28" s="4">
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="6">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="4">
         <v>-6</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="4">
         <v>36</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <v>46</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="4">
         <v>-6</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="4">
         <v>37</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="4">
         <v>41</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="4">
         <v>16</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J29" s="6">
+      <c r="J29" s="4">
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="6">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="4">
         <v>-60</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="4">
         <v>-10</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="4">
         <v>12</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="4">
         <v>-57</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="4">
         <v>-11</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="4">
         <v>13</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="4">
         <v>5</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J30" s="6">
+      <c r="J30" s="4">
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="10" customFormat="1">
-      <c r="A31" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="9">
+    <row r="31" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="7">
         <v>54</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="7">
         <v>14</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="7">
         <v>-26</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="7">
         <v>51</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31" s="7">
         <v>8</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="7">
         <v>-18</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="7">
         <v>5</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J31" s="7">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="K31" s="9"/>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="12">
+        <v>-8</v>
+      </c>
+      <c r="C32" s="12">
+        <v>-68</v>
+      </c>
+      <c r="D32" s="12">
+        <v>56</v>
+      </c>
+      <c r="E32" s="12">
+        <v>-8</v>
+      </c>
+      <c r="F32" s="12">
+        <v>-64</v>
+      </c>
+      <c r="G32" s="12">
+        <v>50</v>
+      </c>
+      <c r="H32" s="12">
+        <v>312</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="12">
+        <v>30</v>
+      </c>
+      <c r="C33" s="12">
+        <v>-58</v>
+      </c>
+      <c r="D33" s="12">
+        <v>50</v>
+      </c>
+      <c r="E33" s="12">
+        <v>31</v>
+      </c>
+      <c r="F33" s="12">
+        <v>-54</v>
+      </c>
+      <c r="G33" s="12">
+        <v>45</v>
+      </c>
+      <c r="H33" s="12">
+        <v>313</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J33" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="12">
+        <v>-14</v>
+      </c>
+      <c r="C34" s="12">
+        <v>-88</v>
+      </c>
+      <c r="D34" s="12">
+        <v>18</v>
+      </c>
+      <c r="E34" s="12">
+        <v>-14</v>
+      </c>
+      <c r="F34" s="12">
+        <v>-84</v>
+      </c>
+      <c r="G34" s="12">
+        <v>19</v>
+      </c>
+      <c r="H34" s="12">
+        <v>66</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="12">
+        <v>38</v>
+      </c>
+      <c r="C35" s="12">
+        <v>-70</v>
+      </c>
+      <c r="D35" s="12">
+        <v>12</v>
+      </c>
+      <c r="E35" s="12">
+        <v>39</v>
+      </c>
+      <c r="F35" s="12">
+        <v>-68</v>
+      </c>
+      <c r="G35" s="12">
+        <v>14</v>
+      </c>
+      <c r="H35" s="12">
+        <v>32</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J35" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="12">
+        <v>40</v>
+      </c>
+      <c r="C36" s="12">
+        <v>-66</v>
+      </c>
+      <c r="D36" s="12">
+        <v>32</v>
+      </c>
+      <c r="E36" s="12">
+        <v>41</v>
+      </c>
+      <c r="F36" s="12">
+        <v>-63</v>
+      </c>
+      <c r="G36" s="12">
+        <v>31</v>
+      </c>
+      <c r="H36" s="12">
+        <v>20</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J36" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="12">
+        <v>20</v>
+      </c>
+      <c r="C37" s="12">
+        <v>-90</v>
+      </c>
+      <c r="D37" s="12">
+        <v>-4</v>
+      </c>
+      <c r="E37" s="12">
+        <v>20</v>
+      </c>
+      <c r="F37" s="12">
+        <v>-88</v>
+      </c>
+      <c r="G37" s="12">
+        <v>1</v>
+      </c>
+      <c r="H37" s="12">
+        <v>365</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J37" s="12">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="12">
+        <v>-32</v>
+      </c>
+      <c r="C38" s="12">
+        <v>-78</v>
+      </c>
+      <c r="D38" s="12">
+        <v>8</v>
+      </c>
+      <c r="E38" s="12">
+        <v>-32</v>
+      </c>
+      <c r="F38" s="12">
+        <v>-76</v>
+      </c>
+      <c r="G38" s="12">
+        <v>11</v>
+      </c>
+      <c r="H38" s="12">
+        <v>38</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J38" s="12">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="12">
+        <v>44</v>
+      </c>
+      <c r="C39" s="12">
+        <v>-74</v>
+      </c>
+      <c r="D39" s="12">
+        <v>0</v>
+      </c>
+      <c r="E39" s="12">
+        <v>45</v>
+      </c>
+      <c r="F39" s="12">
+        <v>-73</v>
+      </c>
+      <c r="G39" s="12">
+        <v>5</v>
+      </c>
+      <c r="H39" s="12">
+        <v>22</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J39" s="12">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="12">
+        <v>-30</v>
+      </c>
+      <c r="C40" s="12">
+        <v>-68</v>
+      </c>
+      <c r="D40" s="12">
+        <v>40</v>
+      </c>
+      <c r="E40" s="12">
+        <v>-30</v>
+      </c>
+      <c r="F40" s="12">
+        <v>-65</v>
+      </c>
+      <c r="G40" s="12">
+        <v>37</v>
+      </c>
+      <c r="H40" s="12">
+        <v>5</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J40" s="12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -1740,11 +2022,6 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1754,14 +2031,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1773,13 +2045,8 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>